<commit_message>
Add remote server shortcuts (show, upload, sync)
</commit_message>
<xml_diff>
--- a/intellij-shortcuts.xlsx
+++ b/intellij-shortcuts.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="137">
   <si>
     <t>Ctrl</t>
   </si>
@@ -576,6 +576,39 @@
   </si>
   <si>
     <r>
+      <t xml:space="preserve">Quick definition </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>/ Optimize imports</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">- </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>/ Surround With Emmet</t>
+    </r>
+  </si>
+  <si>
+    <t>Extract To Parameter</t>
+  </si>
+  <si>
+    <r>
       <rPr>
         <sz val="11"/>
         <color theme="0" tint="-0.499984740745262"/>
@@ -584,22 +617,119 @@
         <charset val="238"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Navigate to super</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Quick definition </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>/ Optimize imports</t>
+      <t>Find file</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> / Find Class</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0" tint="-0.499984740745262"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Find class</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> / New File</t>
+    </r>
+  </si>
+  <si>
+    <t>Scroll up</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Expression Type </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>/ Find Action</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0" tint="-0.499984740745262"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Find Action </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>/ Find all occurrences</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Shrink Selection</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> / Close All Files</t>
+    </r>
+  </si>
+  <si>
+    <t>- / Create block comment</t>
+  </si>
+  <si>
+    <t>Find previous occurrence / -</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Switch Task </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>/ Open Terminal</t>
     </r>
   </si>
   <si>
@@ -614,11 +744,71 @@
         <charset val="238"/>
         <scheme val="minor"/>
       </rPr>
-      <t>/ Surround With Emmet</t>
-    </r>
-  </si>
-  <si>
-    <t>Extract To Parameter</t>
+      <t>/ Open Version Control</t>
+    </r>
+  </si>
+  <si>
+    <t>- / Override Methods</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">- </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>/ Run Task</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">- </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>/ Duplicate to the side</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Parameter Info</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> / Search Everywhere</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">- </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>/ Sync with remote</t>
+    </r>
   </si>
   <si>
     <r>
@@ -630,18 +820,17 @@
         <charset val="238"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Find file</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> / Find Class</t>
+      <t xml:space="preserve">Navigate to super </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>/ Upload to remote</t>
     </r>
   </si>
   <si>
@@ -654,161 +843,17 @@
         <charset val="238"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Find class</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> / New File</t>
-    </r>
-  </si>
-  <si>
-    <t>Scroll up</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Expression Type </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>/ Find Action</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0" tint="-0.499984740745262"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Find Action </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>/ Find all occurrences</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Shrink Selection</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> / Close All Files</t>
-    </r>
-  </si>
-  <si>
-    <t>- / Create block comment</t>
-  </si>
-  <si>
-    <t>Find previous occurrence / -</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Switch Task </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>/ Open Terminal</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">- </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>/ Open Version Control</t>
-    </r>
-  </si>
-  <si>
-    <t>- / Override Methods</t>
-  </si>
-  <si>
-    <t>- / Replace in Files</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">- </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>/ Run Task</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">- </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>/ Duplicate to the side</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Parameter Info</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> / Search Everywhere</t>
+      <t xml:space="preserve">Replace in Files </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>/ Open Remote Hosts</t>
     </r>
   </si>
 </sst>
@@ -1209,15 +1254,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C5" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5" customWidth="1"/>
     <col min="2" max="2" width="40" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="33" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="29.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="26.5703125" style="3" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="35.42578125" customWidth="1"/>
@@ -1247,7 +1292,7 @@
         <v>4</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D2" s="9" t="s">
         <v>85</v>
@@ -1304,7 +1349,7 @@
         <v>68</v>
       </c>
       <c r="D5" s="16" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E5" s="5"/>
     </row>
@@ -1319,7 +1364,7 @@
         <v>69</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E6" s="5"/>
     </row>
@@ -1349,7 +1394,7 @@
         <v>13</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D8" s="9"/>
       <c r="E8" s="5"/>
@@ -1377,7 +1422,7 @@
         <v>60</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D10" s="16" t="s">
         <v>71</v>
@@ -1424,7 +1469,7 @@
         <v>109</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D13" s="11" t="s">
         <v>70</v>
@@ -1453,10 +1498,10 @@
         <v>20</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D15" s="9" t="s">
         <v>88</v>
@@ -1473,7 +1518,7 @@
         <v>74</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D16" s="5" t="s">
         <v>89</v>
@@ -1485,13 +1530,13 @@
         <v>23</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E17" s="5"/>
       <c r="F17" s="3"/>
@@ -1504,7 +1549,7 @@
         <v>64</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D18" s="9"/>
       <c r="E18" s="5" t="s">
@@ -1520,10 +1565,10 @@
         <v>111</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="D19" s="16" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E19" s="5" t="s">
         <v>105</v>
@@ -1561,7 +1606,7 @@
         <v>112</v>
       </c>
       <c r="E21" s="16" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -1569,7 +1614,7 @@
         <v>28</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>117</v>
+        <v>135</v>
       </c>
       <c r="C22" s="8" t="s">
         <v>78</v>
@@ -1600,7 +1645,7 @@
         <v>75</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E24" s="3" t="s">
         <v>107</v>
@@ -1631,7 +1676,7 @@
         <v>80</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>21</v>
+        <v>134</v>
       </c>
       <c r="D26" s="9" t="s">
         <v>94</v>
@@ -1690,7 +1735,7 @@
         <v>40</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C30" s="3" t="s">
         <v>48</v>

</xml_diff>